<commit_message>
Updated MC simulation and fitter
</commit_message>
<xml_diff>
--- a/Documentation/SABR_report.xlsx
+++ b/Documentation/SABR_report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="9340" yWindow="680" windowWidth="24560" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Strike Spread (bps)</t>
   </si>
@@ -118,10 +118,6 @@
   </si>
   <si>
     <t>Black implied volatilities (%) produced by the Milstein scheme for various combinations of beta. For all cases: expiry=10Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nu=0.25, and rho=0.2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -232,13 +228,33 @@
     <t>standard errors for beta=0,0.3,0.5,0.7,1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Black implied volatilities (%) produced by the Euler scheme for various combinations of beta. For all cases: expiry=10Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu=0.25, and rho=0.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu=0, and rho=0.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu=0, and rho=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu=0, and rho=-0.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="183" formatCode="0.000%"/>
+    <numFmt numFmtId="176" formatCode="0.000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -357,7 +373,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,8 +446,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -459,10 +493,16 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -480,11 +520,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="5" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="5" fillId="0" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="5" fillId="0" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="90">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="百分比" xfId="51" builtinId="5"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
@@ -522,6 +559,15 @@
     <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -557,6 +603,15 @@
     <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="88" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -978,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S114"/>
+  <dimension ref="A1:S147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1006,17 +1061,17 @@
     <row r="3" spans="1:19" ht="18" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
       <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1064,7 +1119,7 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7">
@@ -1105,7 +1160,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="24"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="8">
         <v>40</v>
       </c>
@@ -1144,7 +1199,7 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="24"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="8">
         <v>240</v>
       </c>
@@ -1183,7 +1238,7 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="24"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="8">
         <v>480</v>
       </c>
@@ -1222,7 +1277,7 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="24"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="8">
         <v>960</v>
       </c>
@@ -1267,21 +1322,21 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="M10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="8">
@@ -1317,27 +1372,27 @@
       <c r="M11" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="21">
         <v>0.223592653790088</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="23">
         <v>0.17295090075660399</v>
       </c>
-      <c r="P11" s="30">
+      <c r="P11" s="23">
         <v>0.18011695366965599</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="23">
         <v>0.21344433224006701</v>
       </c>
-      <c r="R11" s="30">
+      <c r="R11" s="23">
         <v>4.6955723859909003E-2</v>
       </c>
-      <c r="S11" s="30">
+      <c r="S11" s="23">
         <v>0.50449535842420301</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="26"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="8">
         <v>40</v>
       </c>
@@ -1371,27 +1426,27 @@
       <c r="M12" s="8">
         <v>0.8</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="22">
         <v>1.25550604960179</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="23">
         <v>0.189893903870654</v>
       </c>
-      <c r="P12" s="30">
+      <c r="P12" s="23">
         <v>0.263363759926868</v>
       </c>
-      <c r="Q12" s="30">
+      <c r="Q12" s="23">
         <v>0.316479088633487</v>
       </c>
-      <c r="R12" s="30">
+      <c r="R12" s="23">
         <v>0.43864359217563897</v>
       </c>
-      <c r="S12" s="30">
+      <c r="S12" s="23">
         <v>5.0691499034023</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="26"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="8">
         <v>240</v>
       </c>
@@ -1425,27 +1480,27 @@
       <c r="M13" s="8">
         <v>-0.8</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="22">
         <v>9.86055259008463E-2</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="23">
         <v>5.9375630317443299E-2</v>
       </c>
-      <c r="P13" s="30">
+      <c r="P13" s="23">
         <v>0.11229245503115</v>
       </c>
-      <c r="Q13" s="30">
+      <c r="Q13" s="23">
         <v>5.0904784896088698E-2</v>
       </c>
-      <c r="R13" s="30">
+      <c r="R13" s="23">
         <v>8.7749279180916198E-2</v>
       </c>
-      <c r="S13" s="30">
+      <c r="S13" s="23">
         <v>0.18270548007863199</v>
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="26"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="8">
         <v>480</v>
       </c>
@@ -1478,7 +1533,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="26"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="8">
         <v>960</v>
       </c>
@@ -1524,7 +1579,7 @@
       <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="8">
@@ -1559,7 +1614,7 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="26"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="8">
         <v>40</v>
       </c>
@@ -1592,7 +1647,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="26"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="8">
         <v>240</v>
       </c>
@@ -1625,7 +1680,7 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="26"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="8">
         <v>480</v>
       </c>
@@ -1658,7 +1713,7 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="26"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8">
         <v>960</v>
       </c>
@@ -1704,7 +1759,7 @@
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="8">
@@ -1739,7 +1794,7 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="26"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="8">
         <v>40</v>
       </c>
@@ -1772,7 +1827,7 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="26"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>240</v>
       </c>
@@ -1805,7 +1860,7 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="26"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="8">
         <v>480</v>
       </c>
@@ -1838,7 +1893,7 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="26"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="8">
         <v>960</v>
       </c>
@@ -1884,7 +1939,7 @@
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="8">
@@ -1919,7 +1974,7 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="26"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="8">
         <v>40</v>
       </c>
@@ -1952,7 +2007,7 @@
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="26"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="8">
         <v>240</v>
       </c>
@@ -1985,7 +2040,7 @@
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="26"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="8">
         <v>480</v>
       </c>
@@ -2018,7 +2073,7 @@
       </c>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="27"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="9">
         <v>960</v>
       </c>
@@ -2063,17 +2118,17 @@
     <row r="38" spans="1:11">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
     </row>
     <row r="39" spans="1:11" ht="16" thickBot="1">
       <c r="A39" s="5"/>
@@ -2109,8 +2164,8 @@
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="23" t="s">
-        <v>24</v>
+      <c r="A40" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
@@ -2144,7 +2199,7 @@
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="24"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="8">
         <v>40</v>
       </c>
@@ -2177,7 +2232,7 @@
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="24"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="8">
         <v>240</v>
       </c>
@@ -2210,7 +2265,7 @@
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="24"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="8">
         <v>480</v>
       </c>
@@ -2243,7 +2298,7 @@
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="24"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="8">
         <v>960</v>
       </c>
@@ -2289,8 +2344,8 @@
       <c r="K45" s="15"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="25" t="s">
-        <v>25</v>
+      <c r="A46" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="B46" s="8">
         <v>1</v>
@@ -2324,7 +2379,7 @@
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="26"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="8">
         <v>40</v>
       </c>
@@ -2357,7 +2412,7 @@
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="26"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="8">
         <v>240</v>
       </c>
@@ -2390,7 +2445,7 @@
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="26"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="8">
         <v>480</v>
       </c>
@@ -2423,7 +2478,7 @@
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="26"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="8">
         <v>960</v>
       </c>
@@ -2469,8 +2524,8 @@
       <c r="K51" s="15"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="25" t="s">
-        <v>26</v>
+      <c r="A52" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="B52" s="8">
         <v>1</v>
@@ -2504,7 +2559,7 @@
       </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="26"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="8">
         <v>40</v>
       </c>
@@ -2537,7 +2592,7 @@
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="26"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="8">
         <v>240</v>
       </c>
@@ -2570,7 +2625,7 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="26"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="8">
         <v>480</v>
       </c>
@@ -2603,7 +2658,7 @@
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="26"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="8">
         <v>960</v>
       </c>
@@ -2649,8 +2704,8 @@
       <c r="K57" s="15"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="25" t="s">
-        <v>27</v>
+      <c r="A58" s="29" t="s">
+        <v>26</v>
       </c>
       <c r="B58" s="8">
         <v>1</v>
@@ -2684,7 +2739,7 @@
       </c>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="26"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="8">
         <v>40</v>
       </c>
@@ -2717,7 +2772,7 @@
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="26"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="8">
         <v>240</v>
       </c>
@@ -2750,7 +2805,7 @@
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="26"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="8">
         <v>480</v>
       </c>
@@ -2783,7 +2838,7 @@
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="26"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="8">
         <v>960</v>
       </c>
@@ -2829,8 +2884,8 @@
       <c r="K63" s="15"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="25" t="s">
-        <v>28</v>
+      <c r="A64" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="B64" s="8">
         <v>1</v>
@@ -2864,7 +2919,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="26"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="8">
         <v>40</v>
       </c>
@@ -2897,7 +2952,7 @@
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="26"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="8">
         <v>240</v>
       </c>
@@ -2930,7 +2985,7 @@
       </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="26"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="8">
         <v>480</v>
       </c>
@@ -2963,7 +3018,7 @@
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="27"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="9">
         <v>960</v>
       </c>
@@ -3028,17 +3083,17 @@
     <row r="73" spans="1:11">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26"/>
     </row>
     <row r="74" spans="1:11" ht="16" thickBot="1">
       <c r="A74" s="12"/>
@@ -3074,8 +3129,8 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="23" t="s">
-        <v>29</v>
+      <c r="A75" s="27" t="s">
+        <v>28</v>
       </c>
       <c r="B75" s="7">
         <v>1</v>
@@ -3109,7 +3164,7 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="24"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="8">
         <v>40</v>
       </c>
@@ -3142,7 +3197,7 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="24"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="8">
         <v>240</v>
       </c>
@@ -3175,7 +3230,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="24"/>
+      <c r="A78" s="28"/>
       <c r="B78" s="8">
         <v>480</v>
       </c>
@@ -3208,7 +3263,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="24"/>
+      <c r="A79" s="28"/>
       <c r="B79" s="8">
         <v>960</v>
       </c>
@@ -3254,8 +3309,8 @@
       <c r="K80" s="17"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="25" t="s">
-        <v>30</v>
+      <c r="A81" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="B81" s="8">
         <v>1</v>
@@ -3289,7 +3344,7 @@
       </c>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="26"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="8">
         <v>40</v>
       </c>
@@ -3322,7 +3377,7 @@
       </c>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="26"/>
+      <c r="A83" s="30"/>
       <c r="B83" s="8">
         <v>240</v>
       </c>
@@ -3355,7 +3410,7 @@
       </c>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="26"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="8">
         <v>480</v>
       </c>
@@ -3388,7 +3443,7 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="26"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="8">
         <v>960</v>
       </c>
@@ -3434,8 +3489,8 @@
       <c r="K86" s="17"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="25" t="s">
-        <v>31</v>
+      <c r="A87" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="B87" s="8">
         <v>1</v>
@@ -3469,7 +3524,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="26"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="8">
         <v>40</v>
       </c>
@@ -3502,7 +3557,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="26"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="8">
         <v>240</v>
       </c>
@@ -3535,7 +3590,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="26"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="8">
         <v>480</v>
       </c>
@@ -3568,7 +3623,7 @@
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="26"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="8">
         <v>960</v>
       </c>
@@ -3614,8 +3669,8 @@
       <c r="K92" s="17"/>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="25" t="s">
-        <v>32</v>
+      <c r="A93" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="B93" s="8">
         <v>1</v>
@@ -3649,7 +3704,7 @@
       </c>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="26"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="8">
         <v>40</v>
       </c>
@@ -3682,7 +3737,7 @@
       </c>
     </row>
     <row r="95" spans="1:11">
-      <c r="A95" s="26"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="8">
         <v>240</v>
       </c>
@@ -3715,7 +3770,7 @@
       </c>
     </row>
     <row r="96" spans="1:11">
-      <c r="A96" s="26"/>
+      <c r="A96" s="30"/>
       <c r="B96" s="8">
         <v>480</v>
       </c>
@@ -3748,7 +3803,7 @@
       </c>
     </row>
     <row r="97" spans="1:11">
-      <c r="A97" s="26"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="8">
         <v>960</v>
       </c>
@@ -3794,8 +3849,8 @@
       <c r="K98" s="17"/>
     </row>
     <row r="99" spans="1:11">
-      <c r="A99" s="25" t="s">
-        <v>33</v>
+      <c r="A99" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="B99" s="8">
         <v>1</v>
@@ -3829,7 +3884,7 @@
       </c>
     </row>
     <row r="100" spans="1:11">
-      <c r="A100" s="26"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="8">
         <v>40</v>
       </c>
@@ -3862,7 +3917,7 @@
       </c>
     </row>
     <row r="101" spans="1:11">
-      <c r="A101" s="26"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="8">
         <v>240</v>
       </c>
@@ -3895,7 +3950,7 @@
       </c>
     </row>
     <row r="102" spans="1:11">
-      <c r="A102" s="26"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="8">
         <v>480</v>
       </c>
@@ -3928,7 +3983,7 @@
       </c>
     </row>
     <row r="103" spans="1:11">
-      <c r="A103" s="27"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="9">
         <v>960</v>
       </c>
@@ -3962,27 +4017,27 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="2"/>
-      <c r="B108" s="22" t="s">
+      <c r="B108" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C108" s="22"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="22"/>
-      <c r="G108" s="22"/>
-      <c r="H108" s="22"/>
-      <c r="I108" s="22"/>
-      <c r="J108" s="22"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
+      <c r="I108" s="24"/>
+      <c r="J108" s="24"/>
     </row>
     <row r="109" spans="1:11" ht="16" thickBot="1">
       <c r="A109" s="5"/>
@@ -4019,31 +4074,31 @@
         <v>4</v>
       </c>
       <c r="B110" s="15">
-        <v>37.69</v>
+        <v>31.78</v>
       </c>
       <c r="C110" s="15">
-        <v>31.5</v>
+        <v>28.09</v>
       </c>
       <c r="D110" s="15">
-        <v>26.86</v>
+        <v>25.41</v>
       </c>
       <c r="E110" s="15">
-        <v>24.93</v>
+        <v>24.31</v>
       </c>
       <c r="F110" s="15">
-        <v>23.2</v>
+        <v>23.34</v>
       </c>
       <c r="G110" s="15">
-        <v>21.63</v>
+        <v>22.45</v>
       </c>
       <c r="H110" s="15">
-        <v>20.21</v>
+        <v>21.65</v>
       </c>
       <c r="I110" s="15">
-        <v>17.75</v>
+        <v>20.25</v>
       </c>
       <c r="J110" s="15">
-        <v>15.71</v>
+        <v>19.07</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -4051,31 +4106,31 @@
         <v>18</v>
       </c>
       <c r="B111" s="15">
-        <v>32.35</v>
+        <v>28.11</v>
       </c>
       <c r="C111" s="15">
-        <v>28.42</v>
+        <v>25.91</v>
       </c>
       <c r="D111" s="15">
-        <v>25.24</v>
+        <v>24.22</v>
       </c>
       <c r="E111" s="15">
-        <v>23.86</v>
+        <v>23.51</v>
       </c>
       <c r="F111" s="15">
-        <v>22.59</v>
+        <v>22.87</v>
       </c>
       <c r="G111" s="15">
-        <v>21.42</v>
+        <v>22.29</v>
       </c>
       <c r="H111" s="15">
-        <v>20.329999999999998</v>
+        <v>21.76</v>
       </c>
       <c r="I111" s="15">
-        <v>18.39</v>
+        <v>20.82</v>
       </c>
       <c r="J111" s="15">
-        <v>16.73</v>
+        <v>20.010000000000002</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -4083,31 +4138,31 @@
         <v>19</v>
       </c>
       <c r="B112" s="15">
-        <v>30.88</v>
+        <v>26.72</v>
       </c>
       <c r="C112" s="15">
-        <v>27.61</v>
+        <v>25.18</v>
       </c>
       <c r="D112" s="15">
-        <v>24.95</v>
+        <v>23.98</v>
       </c>
       <c r="E112" s="15">
-        <v>23.78</v>
+        <v>23.47</v>
       </c>
       <c r="F112" s="15">
-        <v>22.71</v>
+        <v>23.01</v>
       </c>
       <c r="G112" s="15">
-        <v>21.72</v>
+        <v>22.58</v>
       </c>
       <c r="H112" s="15">
-        <v>20.8</v>
+        <v>22.19</v>
       </c>
       <c r="I112" s="15">
-        <v>19.16</v>
+        <v>21.5</v>
       </c>
       <c r="J112" s="15">
-        <v>17.75</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -4115,31 +4170,31 @@
         <v>20</v>
       </c>
       <c r="B113" s="15">
-        <v>29.44</v>
+        <v>25.86</v>
       </c>
       <c r="C113" s="15">
-        <v>26.8</v>
+        <v>24.78</v>
       </c>
       <c r="D113" s="15">
-        <v>24.63</v>
+        <v>23.97</v>
       </c>
       <c r="E113" s="15">
-        <v>23.68</v>
+        <v>23.62</v>
       </c>
       <c r="F113" s="15">
-        <v>22.8</v>
+        <v>23.32</v>
       </c>
       <c r="G113" s="15">
-        <v>21.99</v>
+        <v>23.03</v>
       </c>
       <c r="H113" s="15">
-        <v>21.23</v>
+        <v>22.77</v>
       </c>
       <c r="I113" s="15">
-        <v>19.850000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="J113" s="15">
-        <v>18.66</v>
+        <v>21.89</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -4147,35 +4202,678 @@
         <v>21</v>
       </c>
       <c r="B114" s="16">
+        <v>23.98</v>
+      </c>
+      <c r="C114" s="16">
+        <v>23.72</v>
+      </c>
+      <c r="D114" s="16">
+        <v>23.57</v>
+      </c>
+      <c r="E114" s="16">
+        <v>23.51</v>
+      </c>
+      <c r="F114" s="16">
+        <v>23.47</v>
+      </c>
+      <c r="G114" s="16">
+        <v>23.43</v>
+      </c>
+      <c r="H114" s="16">
+        <v>23.4</v>
+      </c>
+      <c r="I114" s="16">
+        <v>23.33</v>
+      </c>
+      <c r="J114" s="16">
+        <v>23.28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="2"/>
+      <c r="B119" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="24"/>
+      <c r="J119" s="24"/>
+    </row>
+    <row r="120" spans="1:10" ht="16" thickBot="1">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5">
+        <v>-150</v>
+      </c>
+      <c r="C120" s="5">
+        <v>-100</v>
+      </c>
+      <c r="D120" s="5">
+        <v>-50</v>
+      </c>
+      <c r="E120" s="5">
+        <v>-25</v>
+      </c>
+      <c r="F120" s="5">
+        <v>0</v>
+      </c>
+      <c r="G120" s="5">
+        <v>25</v>
+      </c>
+      <c r="H120" s="5">
+        <v>50</v>
+      </c>
+      <c r="I120" s="5">
+        <v>100</v>
+      </c>
+      <c r="J120" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="15">
+        <v>31.3</v>
+      </c>
+      <c r="C121" s="15">
+        <v>27.58</v>
+      </c>
+      <c r="D121" s="15">
+        <v>25.04</v>
+      </c>
+      <c r="E121" s="15">
+        <v>23.99</v>
+      </c>
+      <c r="F121" s="15">
+        <v>23.04</v>
+      </c>
+      <c r="G121" s="15">
+        <v>22.19</v>
+      </c>
+      <c r="H121" s="15">
+        <v>21.42</v>
+      </c>
+      <c r="I121" s="15">
+        <v>20.07</v>
+      </c>
+      <c r="J121" s="15">
+        <v>18.920000000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" s="15">
+        <v>28.49</v>
+      </c>
+      <c r="C122" s="15">
+        <v>26.21</v>
+      </c>
+      <c r="D122" s="15">
+        <v>24.46</v>
+      </c>
+      <c r="E122" s="15">
+        <v>23.72</v>
+      </c>
+      <c r="F122" s="15">
+        <v>23.06</v>
+      </c>
+      <c r="G122" s="15">
+        <v>22.45</v>
+      </c>
+      <c r="H122" s="15">
+        <v>21.9</v>
+      </c>
+      <c r="I122" s="15">
+        <v>20.92</v>
+      </c>
+      <c r="J122" s="15">
+        <v>20.07</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123" s="15">
+        <v>27.37</v>
+      </c>
+      <c r="C123" s="15">
+        <v>25.65</v>
+      </c>
+      <c r="D123" s="15">
+        <v>24.36</v>
+      </c>
+      <c r="E123" s="15">
+        <v>23.81</v>
+      </c>
+      <c r="F123" s="15">
+        <v>23.32</v>
+      </c>
+      <c r="G123" s="15">
+        <v>22.87</v>
+      </c>
+      <c r="H123" s="15">
+        <v>22.46</v>
+      </c>
+      <c r="I123" s="15">
+        <v>21.73</v>
+      </c>
+      <c r="J123" s="15">
+        <v>21.09</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" s="15">
+        <v>25.17</v>
+      </c>
+      <c r="C124" s="15">
+        <v>24.28</v>
+      </c>
+      <c r="D124" s="15">
+        <v>23.57</v>
+      </c>
+      <c r="E124" s="15">
+        <v>23.26</v>
+      </c>
+      <c r="F124" s="15">
+        <v>22.98</v>
+      </c>
+      <c r="G124" s="15">
+        <v>22.71</v>
+      </c>
+      <c r="H124" s="15">
+        <v>22.47</v>
+      </c>
+      <c r="I124" s="15">
+        <v>22.04</v>
+      </c>
+      <c r="J124" s="15">
+        <v>21.65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B125" s="16">
+        <v>23.07</v>
+      </c>
+      <c r="C125" s="16">
+        <v>23.09</v>
+      </c>
+      <c r="D125" s="16">
+        <v>23.07</v>
+      </c>
+      <c r="E125" s="16">
+        <v>23.05</v>
+      </c>
+      <c r="F125" s="16">
+        <v>23.04</v>
+      </c>
+      <c r="G125" s="16">
+        <v>23.02</v>
+      </c>
+      <c r="H125" s="16">
+        <v>23</v>
+      </c>
+      <c r="I125" s="16">
+        <v>22.99</v>
+      </c>
+      <c r="J125" s="16">
+        <v>22.97</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="2"/>
+      <c r="B130" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" s="25"/>
+      <c r="D130" s="25"/>
+      <c r="E130" s="25"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="25"/>
+      <c r="H130" s="25"/>
+      <c r="I130" s="25"/>
+      <c r="J130" s="25"/>
+    </row>
+    <row r="131" spans="1:10" ht="16" thickBot="1">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5">
+        <v>-150</v>
+      </c>
+      <c r="C131" s="5">
+        <v>-100</v>
+      </c>
+      <c r="D131" s="5">
+        <v>-50</v>
+      </c>
+      <c r="E131" s="5">
+        <v>-25</v>
+      </c>
+      <c r="F131" s="5">
+        <v>0</v>
+      </c>
+      <c r="G131" s="5">
+        <v>25</v>
+      </c>
+      <c r="H131" s="5">
+        <v>50</v>
+      </c>
+      <c r="I131" s="5">
+        <v>100</v>
+      </c>
+      <c r="J131" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="A132" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="15">
+        <v>31.26</v>
+      </c>
+      <c r="C132" s="15">
+        <v>27.73</v>
+      </c>
+      <c r="D132" s="15">
+        <v>25.12</v>
+      </c>
+      <c r="E132" s="15">
+        <v>24.04</v>
+      </c>
+      <c r="F132" s="15">
+        <v>23.08</v>
+      </c>
+      <c r="G132" s="15">
+        <v>22.21</v>
+      </c>
+      <c r="H132" s="15">
+        <v>21.43</v>
+      </c>
+      <c r="I132" s="15">
+        <v>20.07</v>
+      </c>
+      <c r="J132" s="15">
+        <v>18.91</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="A133" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B133" s="15">
+        <v>28.59</v>
+      </c>
+      <c r="C133" s="15">
+        <v>26.27</v>
+      </c>
+      <c r="D133" s="15">
+        <v>24.49</v>
+      </c>
+      <c r="E133" s="15">
+        <v>23.75</v>
+      </c>
+      <c r="F133" s="15">
+        <v>23.09</v>
+      </c>
+      <c r="G133" s="15">
+        <v>22.48</v>
+      </c>
+      <c r="H133" s="15">
+        <v>21.93</v>
+      </c>
+      <c r="I133" s="15">
+        <v>20.94</v>
+      </c>
+      <c r="J133" s="15">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
+      <c r="A134" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="15">
+        <v>26.56</v>
+      </c>
+      <c r="C134" s="15">
+        <v>25.08</v>
+      </c>
+      <c r="D134" s="15">
+        <v>23.92</v>
+      </c>
+      <c r="E134" s="15">
+        <v>23.43</v>
+      </c>
+      <c r="F134" s="15">
+        <v>22.98</v>
+      </c>
+      <c r="G134" s="15">
+        <v>22.56</v>
+      </c>
+      <c r="H134" s="15">
+        <v>22.18</v>
+      </c>
+      <c r="I134" s="15">
+        <v>21.5</v>
+      </c>
+      <c r="J134" s="15">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
+      <c r="A135" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135" s="15">
+        <v>25.57</v>
+      </c>
+      <c r="C135" s="15">
+        <v>24.56</v>
+      </c>
+      <c r="D135" s="15">
+        <v>23.8</v>
+      </c>
+      <c r="E135" s="15">
+        <v>23.48</v>
+      </c>
+      <c r="F135" s="15">
+        <v>23.18</v>
+      </c>
+      <c r="G135" s="15">
+        <v>22.91</v>
+      </c>
+      <c r="H135" s="15">
+        <v>22.66</v>
+      </c>
+      <c r="I135" s="15">
+        <v>22.2</v>
+      </c>
+      <c r="J135" s="15">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B136" s="16">
+        <v>22.58</v>
+      </c>
+      <c r="C136" s="16">
+        <v>22.76</v>
+      </c>
+      <c r="D136" s="16">
+        <v>22.82</v>
+      </c>
+      <c r="E136" s="16">
+        <v>22.83</v>
+      </c>
+      <c r="F136" s="16">
+        <v>22.83</v>
+      </c>
+      <c r="G136" s="16">
+        <v>22.83</v>
+      </c>
+      <c r="H136" s="16">
+        <v>22.83</v>
+      </c>
+      <c r="I136" s="16">
+        <v>22.82</v>
+      </c>
+      <c r="J136" s="16">
+        <v>22.81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="A140" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" s="2"/>
+      <c r="B141" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141" s="25"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="25"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="25"/>
+      <c r="J141" s="25"/>
+    </row>
+    <row r="142" spans="1:10" ht="16" thickBot="1">
+      <c r="A142" s="5"/>
+      <c r="B142" s="5">
+        <v>-150</v>
+      </c>
+      <c r="C142" s="5">
+        <v>-100</v>
+      </c>
+      <c r="D142" s="5">
+        <v>-50</v>
+      </c>
+      <c r="E142" s="5">
+        <v>-25</v>
+      </c>
+      <c r="F142" s="5">
+        <v>0</v>
+      </c>
+      <c r="G142" s="5">
+        <v>25</v>
+      </c>
+      <c r="H142" s="5">
+        <v>50</v>
+      </c>
+      <c r="I142" s="5">
+        <v>100</v>
+      </c>
+      <c r="J142" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="A143" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="15">
+        <v>37.69</v>
+      </c>
+      <c r="C143" s="15">
+        <v>31.5</v>
+      </c>
+      <c r="D143" s="15">
+        <v>26.86</v>
+      </c>
+      <c r="E143" s="15">
+        <v>24.93</v>
+      </c>
+      <c r="F143" s="15">
+        <v>23.2</v>
+      </c>
+      <c r="G143" s="15">
+        <v>21.63</v>
+      </c>
+      <c r="H143" s="15">
+        <v>20.21</v>
+      </c>
+      <c r="I143" s="15">
+        <v>17.75</v>
+      </c>
+      <c r="J143" s="15">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="A144" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B144" s="15">
+        <v>32.35</v>
+      </c>
+      <c r="C144" s="15">
+        <v>28.42</v>
+      </c>
+      <c r="D144" s="15">
+        <v>25.24</v>
+      </c>
+      <c r="E144" s="15">
+        <v>23.86</v>
+      </c>
+      <c r="F144" s="15">
+        <v>22.59</v>
+      </c>
+      <c r="G144" s="15">
+        <v>21.42</v>
+      </c>
+      <c r="H144" s="15">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="I144" s="15">
+        <v>18.39</v>
+      </c>
+      <c r="J144" s="15">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B145" s="15">
+        <v>30.88</v>
+      </c>
+      <c r="C145" s="15">
+        <v>27.61</v>
+      </c>
+      <c r="D145" s="15">
+        <v>24.95</v>
+      </c>
+      <c r="E145" s="15">
+        <v>23.78</v>
+      </c>
+      <c r="F145" s="15">
+        <v>22.71</v>
+      </c>
+      <c r="G145" s="15">
+        <v>21.72</v>
+      </c>
+      <c r="H145" s="15">
+        <v>20.8</v>
+      </c>
+      <c r="I145" s="15">
+        <v>19.16</v>
+      </c>
+      <c r="J145" s="15">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B146" s="15">
+        <v>29.44</v>
+      </c>
+      <c r="C146" s="15">
+        <v>26.8</v>
+      </c>
+      <c r="D146" s="15">
+        <v>24.63</v>
+      </c>
+      <c r="E146" s="15">
+        <v>23.68</v>
+      </c>
+      <c r="F146" s="15">
+        <v>22.8</v>
+      </c>
+      <c r="G146" s="15">
+        <v>21.99</v>
+      </c>
+      <c r="H146" s="15">
+        <v>21.23</v>
+      </c>
+      <c r="I146" s="15">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="J146" s="15">
+        <v>18.66</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B147" s="16">
         <v>28.12</v>
       </c>
-      <c r="C114" s="16">
+      <c r="C147" s="16">
         <v>26.2</v>
       </c>
-      <c r="D114" s="16">
+      <c r="D147" s="16">
         <v>24.63</v>
       </c>
-      <c r="E114" s="16">
+      <c r="E147" s="16">
         <v>23.94</v>
       </c>
-      <c r="F114" s="16">
+      <c r="F147" s="16">
         <v>23.31</v>
       </c>
-      <c r="G114" s="16">
+      <c r="G147" s="16">
         <v>22.72</v>
       </c>
-      <c r="H114" s="16">
+      <c r="H147" s="16">
         <v>22.17</v>
       </c>
-      <c r="I114" s="16">
+      <c r="I147" s="16">
         <v>21.19</v>
       </c>
-      <c r="J114" s="16">
+      <c r="J147" s="16">
         <v>20.350000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="B130:J130"/>
     <mergeCell ref="O10:S10"/>
     <mergeCell ref="A64:A68"/>
     <mergeCell ref="C3:K3"/>
@@ -4190,7 +4888,7 @@
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A58:A62"/>
     <mergeCell ref="C73:K73"/>
-    <mergeCell ref="B108:J108"/>
+    <mergeCell ref="B141:J141"/>
     <mergeCell ref="A75:A79"/>
     <mergeCell ref="A81:A85"/>
     <mergeCell ref="A87:A91"/>
@@ -4227,15 +4925,15 @@
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="19">
         <v>3.7415316597899998E+21</v>
@@ -4243,7 +4941,7 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="19">
         <v>9.2227982624600002E+21</v>
@@ -4251,7 +4949,7 @@
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="19">
         <v>4.38640345464E+18</v>
@@ -4259,7 +4957,7 @@
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="19">
         <v>2.85251005181E+21</v>
@@ -4267,7 +4965,7 @@
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19">
         <v>2.9021879818499999E+18</v>
@@ -4275,7 +4973,7 @@
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="19">
         <v>2.2299131313400001E+19</v>
@@ -4283,7 +4981,7 @@
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="20">
         <v>1.0185306957799999E+19</v>

</xml_diff>